<commit_message>
Afegir inici de l'informe Inicial
</commit_message>
<xml_diff>
--- a/Organitzacio/Calendari.xlsx
+++ b/Organitzacio/Calendari.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1-Uni 2020-2021\TFG-Joan\Organitzacio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1-Uni 2020-2021\TFG\TFG-Joan\Organitzacio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E540DB-C167-4807-8DDA-CB6E19061056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEF5FA2-32E3-4A8F-BB75-ECB03E890210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15030" yWindow="3780" windowWidth="23370" windowHeight="14940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Setmana</t>
   </si>
@@ -44,6 +44,9 @@
   <si>
     <t xml:space="preserve">Organitzacio general I creacio del calendari I entrada en contacte amb l'SotA </t>
   </si>
+  <si>
+    <t xml:space="preserve">Crear informe inicial  </t>
+  </si>
 </sst>
 </file>
 
@@ -188,11 +191,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -207,6 +208,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,7 +492,7 @@
   <dimension ref="B2:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,130 +502,134 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>3</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="5">
-        <v>5</v>
-      </c>
-      <c r="C6" s="10" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
+        <v>7</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
-        <v>6</v>
-      </c>
-      <c r="C7" s="11" t="s">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="4">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
+      <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="9"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>11</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
+      <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="9"/>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <v>13</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="8"/>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="4">
+      <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="9"/>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
+      <c r="B16" s="3">
         <v>15</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="8"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="4">
+      <c r="B17" s="2">
         <v>16</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="9"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
+      <c r="B18" s="3">
         <v>17</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="4">
+      <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="9"/>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="6">
+      <c r="B20" s="4">
         <v>19</v>
       </c>
-      <c r="C20" s="3"/>
+      <c r="C20" s="8"/>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C21" s="1"/>

</xml_diff>